<commit_message>
fix: update tab name for state
</commit_message>
<xml_diff>
--- a/LWCF/Data/MA_LWCFGrants1965-2011.xlsx
+++ b/LWCF/Data/MA_LWCFGrants1965-2011.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heatherkusmierz/Documents/Files/CodingProjects/LWCF_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heatherkusmierz/GitHub/DataScienceforConservation/LWCF/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF4B79C0-3260-7744-B820-0C6267FE057F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2044E9F7-4C1D-D54B-A0A2-28EA93F0BCB9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{3F8E54BE-A151-6049-967E-B4788891A422}"/>
+    <workbookView xWindow="6680" yWindow="2160" windowWidth="27640" windowHeight="16940" xr2:uid="{3F8E54BE-A151-6049-967E-B4788891A422}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MA" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>

</xml_diff>